<commit_message>
KDP011 ThanhPV print Update
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/KDP011-打刻一覧表_帳票レイアウト（社員別）.xlsx
+++ b/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/KDP011-打刻一覧表_帳票レイアウト（社員別）.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21765" windowHeight="10755"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="帳票テンプレート" sheetId="2" r:id="rId1"/>
@@ -271,11 +271,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -288,7 +288,7 @@
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -432,12 +432,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -447,8 +441,14 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -473,10 +473,12 @@
     <sheetNames>
       <sheetName val="１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ"/>
       <sheetName val="master"/>
+      <sheetName val="Sheet1"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -38431,6 +38433,7 @@
       <sheetName val="収印ﾓﾆﾀｰ"/>
       <sheetName val="収印ﾓﾆﾀｰ.XLS"/>
       <sheetName val="%E5%8F%8E%E5%8D%B0%EF%BE%93%EF%"/>
+      <sheetName val="JOB一覧表"/>
     </sheetNames>
     <definedNames>
       <definedName name="PrintDaicho"/>
@@ -38440,6 +38443,7 @@
       <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -38464,6 +38468,8 @@
     <sheetNames>
       <sheetName val="項目定義書"/>
       <sheetName val="テーブル設計991127"/>
+      <sheetName val="仕切価格"/>
+      <sheetName val="１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1">
@@ -43745,6 +43751,8 @@
         </row>
       </sheetData>
       <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -44040,98 +44048,98 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="12.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.5" style="2" customWidth="1"/>
-    <col min="4" max="5" width="10.625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.75" style="2" customWidth="1"/>
-    <col min="8" max="8" width="17.25" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="2" customWidth="1"/>
+    <col min="4" max="5" width="10.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" style="2" customWidth="1"/>
     <col min="9" max="10" width="10" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12"/>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
+    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
     </row>
-    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
+    <row r="3" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
     </row>
-    <row r="4" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
+    <row r="4" spans="1:11" ht="14.25" customHeight="1">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11">
       <c r="A5" s="4"/>
       <c r="B5" s="6"/>
       <c r="C5" s="5"/>

</xml_diff>

<commit_message>
KDP011 ThanhPV Update Template
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/KDP011-打刻一覧表_帳票レイアウト（社員別）.xlsx
+++ b/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/KDP011-打刻一覧表_帳票レイアウト（社員別）.xlsx
@@ -44055,7 +44055,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -44146,7 +44146,7 @@
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" ht="14.25" customHeight="1">
+    <row r="5" spans="1:11">
       <c r="A5" s="4"/>
       <c r="B5" s="6"/>
       <c r="C5" s="5"/>

</xml_diff>